<commit_message>
pAREI NO DIA 10
</commit_message>
<xml_diff>
--- a/Johnata Pasos.xlsx
+++ b/Johnata Pasos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>Tabela geral Fevereiro</t>
   </si>
@@ -110,9 +110,6 @@
     <t xml:space="preserve">Os demais serviços continua o mesmo valor </t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Jú</t>
   </si>
   <si>
@@ -155,9 +152,6 @@
     <t>CÍLIOS(PRÊMIO) + PÉ + MÃO</t>
   </si>
   <si>
-    <t>PE + MÃO</t>
-  </si>
-  <si>
     <t>TIPO DE PAGAMENTO</t>
   </si>
   <si>
@@ -200,9 +194,6 @@
     <t>Paloma</t>
   </si>
   <si>
-    <t>UNHA-BLINDAGEM</t>
-  </si>
-  <si>
     <t>ESMALTAÇÃO</t>
   </si>
   <si>
@@ -213,6 +204,105 @@
   </si>
   <si>
     <t>BLINDAGEM</t>
+  </si>
+  <si>
+    <t>Lary</t>
+  </si>
+  <si>
+    <t>Jô</t>
+  </si>
+  <si>
+    <t>Bruna Ribeiro</t>
+  </si>
+  <si>
+    <t>JuJu</t>
+  </si>
+  <si>
+    <t>Elineide</t>
+  </si>
+  <si>
+    <t>Mara</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>MANICURE-BLINDAGEM</t>
+  </si>
+  <si>
+    <t>CLIENTE</t>
+  </si>
+  <si>
+    <t>Bruna Secundo</t>
+  </si>
+  <si>
+    <t>Ryana</t>
+  </si>
+  <si>
+    <t>Taila</t>
+  </si>
+  <si>
+    <t>Silvana</t>
+  </si>
+  <si>
+    <t>Forinha</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO + PÉ</t>
+  </si>
+  <si>
+    <t>Bruna</t>
+  </si>
+  <si>
+    <t>Grarnance</t>
+  </si>
+  <si>
+    <t>Zeneide</t>
+  </si>
+  <si>
+    <t>Layane</t>
+  </si>
+  <si>
+    <t>Leticia</t>
+  </si>
+  <si>
+    <t>Verônica</t>
+  </si>
+  <si>
+    <t>ALONGAMENTO-FIBRA + PÉ</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO-FIBRA</t>
+  </si>
+  <si>
+    <t>Beatriz Lourenço</t>
+  </si>
+  <si>
+    <t>Carla Rodrigues</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Tais</t>
+  </si>
+  <si>
+    <t>Jamile</t>
+  </si>
+  <si>
+    <t>MÃO-PÉ</t>
+  </si>
+  <si>
+    <t>MANUTENÇÃO-FIBRA + PÉ</t>
+  </si>
+  <si>
+    <t>SOBRANCELHA</t>
+  </si>
+  <si>
+    <t>PÉ + MÃO + SOBRANCELHA</t>
   </si>
 </sst>
 </file>
@@ -251,11 +341,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:O25"/>
+  <dimension ref="B3:O61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +641,7 @@
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -560,14 +654,14 @@
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -576,7 +670,7 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="O4" t="s">
         <v>11</v>
@@ -593,13 +687,13 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="3">
         <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O5" t="s">
         <v>12</v>
@@ -616,13 +710,13 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3">
         <v>130</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O6" t="s">
         <v>13</v>
@@ -639,13 +733,13 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="3">
         <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O7" t="s">
         <v>14</v>
@@ -662,13 +756,13 @@
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3">
         <v>150</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O8" t="s">
         <v>15</v>
@@ -685,13 +779,13 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" s="3">
         <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O9" t="s">
         <v>16</v>
@@ -705,16 +799,16 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3">
         <v>57</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O10" t="s">
         <v>17</v>
@@ -728,16 +822,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="3">
         <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O11" t="s">
         <v>18</v>
@@ -751,16 +845,16 @@
         <v>0.625</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="3">
         <v>55</v>
       </c>
       <c r="G12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O12" t="s">
         <v>19</v>
@@ -774,16 +868,16 @@
         <v>0.64583333333333337</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F13" s="3">
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O13" t="s">
         <v>20</v>
@@ -797,16 +891,16 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F14" s="3">
         <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O14" t="s">
         <v>21</v>
@@ -820,16 +914,16 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F15" s="3">
         <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="O15" t="s">
         <v>22</v>
@@ -843,16 +937,16 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F16" s="3">
         <v>100</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O16" t="s">
         <v>23</v>
@@ -866,13 +960,16 @@
         <v>0.41666666666666669</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F17" s="3">
         <v>90</v>
+      </c>
+      <c r="G17" t="s">
+        <v>45</v>
       </c>
       <c r="O17" t="s">
         <v>24</v>
@@ -886,13 +983,16 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3">
         <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
       </c>
       <c r="O18" t="s">
         <v>25</v>
@@ -906,13 +1006,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F19" s="3">
         <v>55</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
       </c>
       <c r="O19" t="s">
         <v>26</v>
@@ -926,13 +1029,16 @@
         <v>0.54166666666666663</v>
       </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F20" s="3">
         <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
@@ -943,13 +1049,16 @@
         <v>0.625</v>
       </c>
       <c r="D21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F21" s="3">
         <v>65</v>
+      </c>
+      <c r="G21" t="s">
+        <v>45</v>
       </c>
       <c r="O21" t="s">
         <v>27</v>
@@ -963,13 +1072,16 @@
         <v>0.625</v>
       </c>
       <c r="D22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F22" s="3">
         <v>120</v>
+      </c>
+      <c r="G22" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -980,13 +1092,16 @@
         <v>0.625</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F23" s="3">
         <v>160</v>
+      </c>
+      <c r="G23" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
@@ -997,13 +1112,16 @@
         <v>0.6875</v>
       </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="3">
         <v>55</v>
+      </c>
+      <c r="G24" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
@@ -1014,13 +1132,682 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="D25" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F25" s="3">
         <v>90</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>45326</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="3">
+        <v>65</v>
+      </c>
+      <c r="G26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>45326</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="3">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>45326</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="D28" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="3">
+        <v>130</v>
+      </c>
+      <c r="G28" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>45326</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="3">
+        <v>50</v>
+      </c>
+      <c r="G29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>45328</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D30" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="3">
+        <v>30</v>
+      </c>
+      <c r="G30" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>45328</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D31" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="3">
+        <v>50</v>
+      </c>
+      <c r="G31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>45328</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D32" t="s">
+        <v>63</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="3">
+        <v>32</v>
+      </c>
+      <c r="G32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>45328</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="3">
+        <v>60</v>
+      </c>
+      <c r="G33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>45328</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="3">
+        <v>135</v>
+      </c>
+      <c r="G34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="3">
+        <v>60</v>
+      </c>
+      <c r="G35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" t="s">
+        <v>35</v>
+      </c>
+      <c r="F36" s="3">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="3">
+        <v>30</v>
+      </c>
+      <c r="G37" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="3">
+        <v>30</v>
+      </c>
+      <c r="G38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D39" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="3">
+        <v>150</v>
+      </c>
+      <c r="G39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D40" t="s">
+        <v>71</v>
+      </c>
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="3">
+        <v>50</v>
+      </c>
+      <c r="G40" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+      <c r="E41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="3">
+        <v>50</v>
+      </c>
+      <c r="G41" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="3">
+        <v>160</v>
+      </c>
+      <c r="G42" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>45330</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+      <c r="F43" s="3">
+        <v>30</v>
+      </c>
+      <c r="G43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D44" t="s">
+        <v>76</v>
+      </c>
+      <c r="E44" t="s">
+        <v>37</v>
+      </c>
+      <c r="F44" s="3">
+        <v>125</v>
+      </c>
+      <c r="G44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="D45" t="s">
+        <v>77</v>
+      </c>
+      <c r="E45" t="s">
+        <v>35</v>
+      </c>
+      <c r="F45" s="3">
+        <v>25</v>
+      </c>
+      <c r="G45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D46" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" t="s">
+        <v>82</v>
+      </c>
+      <c r="F46" s="3">
+        <v>240</v>
+      </c>
+      <c r="G46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D47" t="s">
+        <v>79</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="3">
+        <v>50</v>
+      </c>
+      <c r="G47" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+      <c r="E48" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="3">
+        <v>32</v>
+      </c>
+      <c r="G48" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D49" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="3">
+        <v>25</v>
+      </c>
+      <c r="G49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+      <c r="E50" t="s">
+        <v>83</v>
+      </c>
+      <c r="F50" s="3">
+        <v>150</v>
+      </c>
+      <c r="G50" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D51" t="s">
+        <v>32</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+      <c r="F51" s="3">
+        <v>25</v>
+      </c>
+      <c r="G51" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>45331</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52" s="3">
+        <v>50</v>
+      </c>
+      <c r="G52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D53" t="s">
+        <v>84</v>
+      </c>
+      <c r="E53" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D54" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="D55" t="s">
+        <v>60</v>
+      </c>
+      <c r="E55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D56" t="s">
+        <v>85</v>
+      </c>
+      <c r="E56" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D59" t="s">
+        <v>86</v>
+      </c>
+      <c r="E59" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D60" t="s">
+        <v>87</v>
+      </c>
+      <c r="E60" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>45332</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D61" t="s">
+        <v>88</v>
+      </c>
+      <c r="E61" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>